<commit_message>
Atualização e finalização do projeto Dashboard com Excel.
</commit_message>
<xml_diff>
--- a/Assets/Assets.xlsx
+++ b/Assets/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projetos Git\Criando-um-Dashboard-de-Vendas-do-Xbox\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0DDE7-0477-4D6C-A0D8-6E1A897410D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ABF4D8-E08F-4591-A7AD-E7378E0DFE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="19200" windowHeight="14640" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="19200" windowHeight="14640" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
     <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
@@ -1059,8 +1059,8 @@
   </sheetPr>
   <dimension ref="B3:P21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,26 +1226,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -1500,26 +1480,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1536,4 +1517,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>